<commit_message>
checking in before major changes
</commit_message>
<xml_diff>
--- a/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
+++ b/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
@@ -20,15 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">External_ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Part Type Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z.Sandbox.HWDBUnitTest.snork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External ID</t>
   </si>
   <si>
     <t xml:space="preserve">Serial Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institution ID</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacturer</t>
@@ -154,17 +169,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -184,20 +203,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ2"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.68"/>
@@ -213,68 +232,160 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B4" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>14</v>
+      <c r="J7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updating "Docket" and "Sheet" objects
</commit_message>
<xml_diff>
--- a/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
+++ b/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">Part Type Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Institution ID</t>
   </si>
   <si>
     <t xml:space="preserve">Z.Sandbox.HWDBUnitTest.snork</t>
@@ -37,7 +37,10 @@
     <t xml:space="preserve">Manufacturer ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Institution ID</t>
+    <t xml:space="preserve">Encoder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SiPM Item</t>
   </si>
   <si>
     <t xml:space="preserve">External ID</t>
@@ -203,13 +206,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
@@ -281,7 +284,7 @@
     </row>
     <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>59</v>
@@ -298,8 +301,12 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -312,79 +319,94 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="K7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C8" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="F8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="K8" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Changes to Encoder and Sheet
</commit_message>
<xml_diff>
--- a/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
+++ b/test/HWDBUploader/SystemTest/002/SiPM-item-manifest.xlsx
@@ -20,21 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">Part Type Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z.Sandbox.HWDBUnitTest.snork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer ID</t>
+  </si>
   <si>
     <t xml:space="preserve">Institution ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z.Sandbox.HWDBUnitTest.snork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheet Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturer ID</t>
   </si>
   <si>
     <t xml:space="preserve">Encoder</t>
@@ -212,7 +215,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.97"/>
@@ -284,7 +287,7 @@
     </row>
     <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>59</v>
@@ -302,10 +305,10 @@
     </row>
     <row r="5" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -334,37 +337,37 @@
     </row>
     <row r="7" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AMJ7" s="0"/>
     </row>
@@ -379,10 +382,10 @@
         <v>48</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>9</v>
@@ -394,10 +397,10 @@
         <v>171</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>